<commit_message>
Completed insertion of data and handled duplicates and date and time errors
</commit_message>
<xml_diff>
--- a/static/demo excel/test1.xlsx
+++ b/static/demo excel/test1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreyas1.Sawant\Desktop\PrintDesk\static\demo excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soham3.Patil\Desktop\PrintDesk\static\demo excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9BF85C4-3FED-46B1-9BC4-405DD7813AB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8242EC8F-224A-4E22-AA77-037128CDEDCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{0198FBDB-EF18-4566-9FDD-9DF83F9E478F}"/>
   </bookViews>
@@ -340,327 +340,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -16297,7 +15977,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16316,10 +15996,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>

</xml_diff>